<commit_message>
Chnages done for madison site
</commit_message>
<xml_diff>
--- a/MadisionIslandSite/src/main/resources/Madison.xlsx
+++ b/MadisionIslandSite/src/main/resources/Madison.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16095" windowHeight="6180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16110" windowHeight="6180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="1" r:id="rId1"/>
     <sheet name="login" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A5:J22"/>
+  <oleSize ref="A1:I18"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -59,7 +59,7 @@
     <t>saireddy</t>
   </si>
   <si>
-    <t>saivara78901234679@gmail.com</t>
+    <t>saivara34256@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -390,8 +390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>